<commit_message>
Forgot to save excel file.
</commit_message>
<xml_diff>
--- a/sp500values.xlsx
+++ b/sp500values.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxlascombe/Documents/School/Columbia/Senior Spring/finance/FinalProject/MagicFormulaInvesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C61D4384-EF02-DE4C-889C-FDDE424999C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8845F2A2-EFD2-C44B-8F61-CFB5592A300D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WRDS" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WRDS!$A$1:$E$1</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
   <si>
     <t>Global Index Key - Index Monthly</t>
   </si>
@@ -55,12 +56,18 @@
   <si>
     <t>Year Month</t>
   </si>
+  <si>
+    <t>Magic Formula</t>
+  </si>
+  <si>
+    <t>S&amp;P 500</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -73,6 +80,13 @@
       <sz val="12"/>
       <color indexed="9"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -101,11 +115,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -121,6 +137,1154 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Magic Formula</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>989610</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>968972</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>949223</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>945373</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>948098</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>911659</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>895880</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>898780</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>881058</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>865951</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>853060</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>827517</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>818510</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>813358</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>803863</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>778403</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>780579</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>778483</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>800972</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>828444</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>812893</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>810357</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>854689</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>862428</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>866796</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>865496</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>887525</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>908567</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>914987</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>906327</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>894870</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>903446</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>903446</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>895053</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>894068</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-81F8-8849-AAFB-6844940CAA91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>S&amp;P 500</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1438.24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1406.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1420.86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1482.37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1530.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1503.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1455.27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1473.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1526.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1549.38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1481.14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1468.36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1378.55</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1330.63</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1322.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1385.59</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1400.38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1280</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1267.3800000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1282.83</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1166.3599999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>968.75</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>896.24</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>903.25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>825.88</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>735.09</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>797.87</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>872.81</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>919.14</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>919.32</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>987.48</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1020.62</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1057.08</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1036.19</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1095.6300000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1115.0999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-81F8-8849-AAFB-6844940CAA91}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="314553744"/>
+        <c:axId val="313930384"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="314553744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="313930384"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="313930384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="314553744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AB856B2-06B2-3447-911F-BB134AB20620}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,11 +1586,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1120,4 +2284,320 @@
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06E654E-58A5-7E40-8577-25EC76FE7BFE}">
+  <dimension ref="A1:B37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="B2">
+        <v>1438.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>989610</v>
+      </c>
+      <c r="B3">
+        <v>1406.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>968972</v>
+      </c>
+      <c r="B4">
+        <v>1420.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>949223</v>
+      </c>
+      <c r="B5">
+        <v>1482.37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>945373</v>
+      </c>
+      <c r="B6">
+        <v>1530.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>948098</v>
+      </c>
+      <c r="B7">
+        <v>1503.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>911659</v>
+      </c>
+      <c r="B8">
+        <v>1455.27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>895880</v>
+      </c>
+      <c r="B9">
+        <v>1473.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>898780</v>
+      </c>
+      <c r="B10">
+        <v>1526.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>881058</v>
+      </c>
+      <c r="B11">
+        <v>1549.38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>865951</v>
+      </c>
+      <c r="B12">
+        <v>1481.14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>853060</v>
+      </c>
+      <c r="B13">
+        <v>1468.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>827517</v>
+      </c>
+      <c r="B14">
+        <v>1378.55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>818510</v>
+      </c>
+      <c r="B15">
+        <v>1330.63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>813358</v>
+      </c>
+      <c r="B16">
+        <v>1322.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>803863</v>
+      </c>
+      <c r="B17">
+        <v>1385.59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>778403</v>
+      </c>
+      <c r="B18">
+        <v>1400.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>780579</v>
+      </c>
+      <c r="B19">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>778483</v>
+      </c>
+      <c r="B20">
+        <v>1267.3800000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>800972</v>
+      </c>
+      <c r="B21">
+        <v>1282.83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>828444</v>
+      </c>
+      <c r="B22">
+        <v>1166.3599999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>812893</v>
+      </c>
+      <c r="B23">
+        <v>968.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>810357</v>
+      </c>
+      <c r="B24">
+        <v>896.24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>854689</v>
+      </c>
+      <c r="B25">
+        <v>903.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>862428</v>
+      </c>
+      <c r="B26">
+        <v>825.88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>866796</v>
+      </c>
+      <c r="B27">
+        <v>735.09</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>865496</v>
+      </c>
+      <c r="B28">
+        <v>797.87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>887525</v>
+      </c>
+      <c r="B29">
+        <v>872.81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>908567</v>
+      </c>
+      <c r="B30">
+        <v>919.14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>914987</v>
+      </c>
+      <c r="B31">
+        <v>919.32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>906327</v>
+      </c>
+      <c r="B32">
+        <v>987.48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>894870</v>
+      </c>
+      <c r="B33">
+        <v>1020.62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>903446</v>
+      </c>
+      <c r="B34">
+        <v>1057.08</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>903446</v>
+      </c>
+      <c r="B35">
+        <v>1036.19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>895053</v>
+      </c>
+      <c r="B36">
+        <v>1095.6300000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>894068</v>
+      </c>
+      <c r="B37">
+        <v>1115.0999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding excel file with graphs
</commit_message>
<xml_diff>
--- a/sp500values.xlsx
+++ b/sp500values.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxlascombe/Documents/School/Columbia/Senior Spring/finance/FinalProject/MagicFormulaInvesting/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescogrechi/Google Drive/Columbia/Senior Year/Spring Semester/FinancialMath/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8845F2A2-EFD2-C44B-8F61-CFB5592A300D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F89B6D0-3C74-2945-9EF2-ACEA9033AFB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WRDS" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,33 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WRDS!$A$1:$E$1</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$D$2:$D$37</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$E$2:$E$37</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$D$2:$D$37</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$E$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$E$2:$E$37</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$2:$C$37</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$A$2:$A$37</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$2:$B$37</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$2:$C$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
   <si>
     <t>Global Index Key - Index Monthly</t>
   </si>
@@ -57,17 +75,26 @@
     <t>Year Month</t>
   </si>
   <si>
-    <t>Magic Formula</t>
+    <t>S&amp;P 500</t>
   </si>
   <si>
-    <t>S&amp;P 500</t>
+    <t>Portfolio Value</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Portfolio Return</t>
+  </si>
+  <si>
+    <t>Market Return</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -88,8 +115,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +144,14 @@
         <bgColor indexed="18"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -111,20 +159,159 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -154,6 +341,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Quarterly Portfolio</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> &amp; S&amp;P 500 Values </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -194,11 +411,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Magic Formula</c:v>
+                  <c:v>Portfolio Value</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -215,9 +432,126 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39173</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39234</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39264</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39295</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39356</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39387</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39448</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39479</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39508</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39569</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39661</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39692</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39722</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39753</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39783</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39814</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39845</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39873</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39904</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39934</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39965</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39995</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40087</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40118</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:f>Sheet1!$B$2:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -335,16 +669,32 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-81F8-8849-AAFB-6844940CAA91}"/>
+              <c16:uniqueId val="{00000000-7DB8-D241-89AF-29A949DADACE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="817946111"/>
+        <c:axId val="817947743"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -365,9 +715,126 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39173</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39234</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39264</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39295</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39356</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39387</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39448</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39479</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39508</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39569</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39661</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39692</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39722</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39753</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39783</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39814</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39845</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39873</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39904</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39934</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39965</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39995</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40087</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40118</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$37</c:f>
+              <c:f>Sheet1!$C$2:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -485,7 +952,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-81F8-8849-AAFB-6844940CAA91}"/>
+              <c16:uniqueId val="{00000001-7DB8-D241-89AF-29A949DADACE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -497,18 +964,20 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="314553744"/>
-        <c:axId val="313930384"/>
+        <c:axId val="776876799"/>
+        <c:axId val="776874367"/>
       </c:lineChart>
-      <c:catAx>
-        <c:axId val="314553744"/>
+      <c:dateAx>
+        <c:axId val="817946111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -544,15 +1013,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313930384"/>
+        <c:crossAx val="817947743"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
       <c:valAx>
-        <c:axId val="313930384"/>
+        <c:axId val="817947743"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +1071,876 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314553744"/>
+        <c:crossAx val="817946111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="776874367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="776876799"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dateAx>
+        <c:axId val="776876799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="776874367"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Quarterly</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Portfolio &amp; Market Returns </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Portfolio Return</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39173</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39234</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39264</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39295</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39356</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39387</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39448</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39479</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39508</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39569</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39661</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39692</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39722</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39753</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39783</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39814</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39845</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39873</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39904</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39934</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39965</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39995</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40087</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40118</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.039E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.1028E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.0777000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.4627000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.1901999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.8341000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.10412</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.10122</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.11894200000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.134049</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.14693999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.172483</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.18149000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.186642</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.19613700000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.22159699999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.219421</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.22151699999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.19902800000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.17155599999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.187107</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.18964300000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.145311</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.137572</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.13320399999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.13450400000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.11247500000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-9.1433E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-8.5013000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-9.3673000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.10513</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-9.6554000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-9.6554000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.104947</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.105932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F130-4243-8812-D57B314CECCE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Market Return</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39173</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>39234</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39264</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39295</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>39326</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>39356</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39387</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39448</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>39479</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39508</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>39569</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39661</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39692</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>39722</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>39753</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>39783</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>39814</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>39845</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>39873</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>39904</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>39934</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>39965</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>39995</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>40026</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40087</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>40118</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.1846145288686222E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.2084214039381543E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0683335187451248E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4231282678829604E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5270608521526243E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1840861052397355E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4856769384803648E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.1540493937034146E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.7275002781177063E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9828123261764442E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0942262765602328E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-4.1502113694515556E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-7.482061408388023E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-8.0334297474691257E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-3.660724218489271E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-2.6323840249193389E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.11002336188675048</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.11879797530314823</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.10805567916342201</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.18903660028924249</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.32643369674046058</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.3768494827010791</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.37197547001891201</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.42577038602736678</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.48889615085104016</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.44524557792857938</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.39314022694404277</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.36092724440983426</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.36080209144509956</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.31341083546556903</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.29036878406941818</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.26501835576816113</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.27954305261986867</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.23821476248748463</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.22467738346868402</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F130-4243-8812-D57B314CECCE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="818377199"/>
+        <c:axId val="818085055"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="818377199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="818085055"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="818085055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="818377199"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -730,6 +2067,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1246,27 +2623,530 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2AB856B2-06B2-3447-911F-BB134AB20620}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA52105F-5855-2B4D-BA59-37F215624900}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1279,6 +3159,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C18499-8985-4E49-ACDA-97D301417F95}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1587,10 +3503,10 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:C37"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2288,312 +4204,719 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06E654E-58A5-7E40-8577-25EC76FE7BFE}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>39083</v>
+      </c>
+      <c r="B2" s="5">
         <v>1000000</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="6">
         <v>1438.24</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="D2" s="12">
+        <f>(B2-$B$2)/$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <f>(C2-$C$2)/$C$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>39114</v>
+      </c>
+      <c r="B3" s="5">
         <v>989610</v>
       </c>
-      <c r="B3">
+      <c r="C3" s="6">
         <v>1406.82</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="D3" s="12">
+        <f t="shared" ref="D3:D37" si="0">(B3-$B$2)/$B$2</f>
+        <v>-1.039E-2</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" ref="E3:E37" si="1">(C3-$C$2)/$C$2</f>
+        <v>-2.1846145288686222E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>39142</v>
+      </c>
+      <c r="B4" s="5">
         <v>968972</v>
       </c>
-      <c r="B4">
+      <c r="C4" s="6">
         <v>1420.86</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="D4" s="12">
+        <f t="shared" si="0"/>
+        <v>-3.1028E-2</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="1"/>
+        <v>-1.2084214039381543E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>39173</v>
+      </c>
+      <c r="B5" s="5">
         <v>949223</v>
       </c>
-      <c r="B5">
+      <c r="C5" s="6">
         <v>1482.37</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="D5" s="12">
+        <f t="shared" si="0"/>
+        <v>-5.0777000000000003E-2</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="1"/>
+        <v>3.0683335187451248E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>39203</v>
+      </c>
+      <c r="B6" s="5">
         <v>945373</v>
       </c>
-      <c r="B6">
+      <c r="C6" s="6">
         <v>1530.62</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="D6" s="12">
+        <f t="shared" si="0"/>
+        <v>-5.4627000000000002E-2</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="1"/>
+        <v>6.4231282678829604E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>39234</v>
+      </c>
+      <c r="B7" s="5">
         <v>948098</v>
       </c>
-      <c r="B7">
+      <c r="C7" s="6">
         <v>1503.35</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="D7" s="12">
+        <f t="shared" si="0"/>
+        <v>-5.1901999999999997E-2</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="1"/>
+        <v>4.5270608521526243E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>39264</v>
+      </c>
+      <c r="B8" s="5">
         <v>911659</v>
       </c>
-      <c r="B8">
+      <c r="C8" s="6">
         <v>1455.27</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="D8" s="12">
+        <f t="shared" si="0"/>
+        <v>-8.8341000000000003E-2</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="1"/>
+        <v>1.1840861052397355E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>39295</v>
+      </c>
+      <c r="B9" s="5">
         <v>895880</v>
       </c>
-      <c r="B9">
+      <c r="C9" s="6">
         <v>1473.99</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="D9" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.10412</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="1"/>
+        <v>2.4856769384803648E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>39326</v>
+      </c>
+      <c r="B10" s="5">
         <v>898780</v>
       </c>
-      <c r="B10">
+      <c r="C10" s="6">
         <v>1526.75</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="D10" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.10122</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="1"/>
+        <v>6.1540493937034146E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>39356</v>
+      </c>
+      <c r="B11" s="5">
         <v>881058</v>
       </c>
-      <c r="B11">
+      <c r="C11" s="6">
         <v>1549.38</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="D11" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.11894200000000001</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="1"/>
+        <v>7.7275002781177063E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>39387</v>
+      </c>
+      <c r="B12" s="5">
         <v>865951</v>
       </c>
-      <c r="B12">
+      <c r="C12" s="6">
         <v>1481.14</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.134049</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="1"/>
+        <v>2.9828123261764442E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>39417</v>
+      </c>
+      <c r="B13" s="5">
         <v>853060</v>
       </c>
-      <c r="B13">
+      <c r="C13" s="6">
         <v>1468.36</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="D13" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.14693999999999999</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="1"/>
+        <v>2.0942262765602328E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>39448</v>
+      </c>
+      <c r="B14" s="5">
         <v>827517</v>
       </c>
-      <c r="B14">
+      <c r="C14" s="6">
         <v>1378.55</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="D14" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.172483</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="1"/>
+        <v>-4.1502113694515556E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>39479</v>
+      </c>
+      <c r="B15" s="5">
         <v>818510</v>
       </c>
-      <c r="B15">
+      <c r="C15" s="6">
         <v>1330.63</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="D15" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.18149000000000001</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="1"/>
+        <v>-7.482061408388023E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>39508</v>
+      </c>
+      <c r="B16" s="5">
         <v>813358</v>
       </c>
-      <c r="B16">
+      <c r="C16" s="6">
         <v>1322.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="D16" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.186642</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="1"/>
+        <v>-8.0334297474691257E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>39539</v>
+      </c>
+      <c r="B17" s="5">
         <v>803863</v>
       </c>
-      <c r="B17">
+      <c r="C17" s="6">
         <v>1385.59</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="D17" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.19613700000000001</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="1"/>
+        <v>-3.660724218489271E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>39569</v>
+      </c>
+      <c r="B18" s="5">
         <v>778403</v>
       </c>
-      <c r="B18">
+      <c r="C18" s="6">
         <v>1400.38</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="D18" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.22159699999999999</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="1"/>
+        <v>-2.6323840249193389E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>39600</v>
+      </c>
+      <c r="B19" s="5">
         <v>780579</v>
       </c>
-      <c r="B19">
+      <c r="C19" s="6">
         <v>1280</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="D19" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.219421</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.11002336188675048</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>39630</v>
+      </c>
+      <c r="B20" s="5">
         <v>778483</v>
       </c>
-      <c r="B20">
+      <c r="C20" s="6">
         <v>1267.3800000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="D20" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.22151699999999999</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.11879797530314823</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>39661</v>
+      </c>
+      <c r="B21" s="5">
         <v>800972</v>
       </c>
-      <c r="B21">
+      <c r="C21" s="6">
         <v>1282.83</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="D21" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.19902800000000001</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.10805567916342201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>39692</v>
+      </c>
+      <c r="B22" s="5">
         <v>828444</v>
       </c>
-      <c r="B22">
+      <c r="C22" s="6">
         <v>1166.3599999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="D22" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.17155599999999999</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.18903660028924249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>39722</v>
+      </c>
+      <c r="B23" s="5">
         <v>812893</v>
       </c>
-      <c r="B23">
+      <c r="C23" s="6">
         <v>968.75</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="D23" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.187107</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.32643369674046058</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>39753</v>
+      </c>
+      <c r="B24" s="5">
         <v>810357</v>
       </c>
-      <c r="B24">
+      <c r="C24" s="6">
         <v>896.24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="D24" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.18964300000000001</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.3768494827010791</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
+        <v>39783</v>
+      </c>
+      <c r="B25" s="5">
         <v>854689</v>
       </c>
-      <c r="B25">
+      <c r="C25" s="6">
         <v>903.25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="D25" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.145311</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.37197547001891201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>39814</v>
+      </c>
+      <c r="B26" s="5">
         <v>862428</v>
       </c>
-      <c r="B26">
+      <c r="C26" s="6">
         <v>825.88</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="D26" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.137572</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.42577038602736678</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>39845</v>
+      </c>
+      <c r="B27" s="5">
         <v>866796</v>
       </c>
-      <c r="B27">
+      <c r="C27" s="6">
         <v>735.09</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="D27" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.13320399999999999</v>
+      </c>
+      <c r="E27" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.48889615085104016</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="10">
+        <v>39873</v>
+      </c>
+      <c r="B28" s="5">
         <v>865496</v>
       </c>
-      <c r="B28">
+      <c r="C28" s="6">
         <v>797.87</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="D28" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.13450400000000001</v>
+      </c>
+      <c r="E28" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.44524557792857938</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>39904</v>
+      </c>
+      <c r="B29" s="5">
         <v>887525</v>
       </c>
-      <c r="B29">
+      <c r="C29" s="6">
         <v>872.81</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="D29" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.11247500000000001</v>
+      </c>
+      <c r="E29" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.39314022694404277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="10">
+        <v>39934</v>
+      </c>
+      <c r="B30" s="5">
         <v>908567</v>
       </c>
-      <c r="B30">
+      <c r="C30" s="6">
         <v>919.14</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="D30" s="12">
+        <f t="shared" si="0"/>
+        <v>-9.1433E-2</v>
+      </c>
+      <c r="E30" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.36092724440983426</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="10">
+        <v>39965</v>
+      </c>
+      <c r="B31" s="5">
         <v>914987</v>
       </c>
-      <c r="B31">
+      <c r="C31" s="6">
         <v>919.32</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="D31" s="12">
+        <f t="shared" si="0"/>
+        <v>-8.5013000000000005E-2</v>
+      </c>
+      <c r="E31" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.36080209144509956</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="10">
+        <v>39995</v>
+      </c>
+      <c r="B32" s="5">
         <v>906327</v>
       </c>
-      <c r="B32">
+      <c r="C32" s="6">
         <v>987.48</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="D32" s="12">
+        <f t="shared" si="0"/>
+        <v>-9.3673000000000006E-2</v>
+      </c>
+      <c r="E32" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.31341083546556903</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="10">
+        <v>40026</v>
+      </c>
+      <c r="B33" s="5">
         <v>894870</v>
       </c>
-      <c r="B33">
+      <c r="C33" s="6">
         <v>1020.62</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="D33" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.10513</v>
+      </c>
+      <c r="E33" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.29036878406941818</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="10">
+        <v>40057</v>
+      </c>
+      <c r="B34" s="5">
         <v>903446</v>
       </c>
-      <c r="B34">
+      <c r="C34" s="6">
         <v>1057.08</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="D34" s="12">
+        <f t="shared" si="0"/>
+        <v>-9.6554000000000001E-2</v>
+      </c>
+      <c r="E34" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.26501835576816113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>40087</v>
+      </c>
+      <c r="B35" s="5">
         <v>903446</v>
       </c>
-      <c r="B35">
+      <c r="C35" s="6">
         <v>1036.19</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="D35" s="12">
+        <f t="shared" si="0"/>
+        <v>-9.6554000000000001E-2</v>
+      </c>
+      <c r="E35" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.27954305261986867</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="10">
+        <v>40118</v>
+      </c>
+      <c r="B36" s="5">
         <v>895053</v>
       </c>
-      <c r="B36">
+      <c r="C36" s="6">
         <v>1095.6300000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+      <c r="D36" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.104947</v>
+      </c>
+      <c r="E36" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.23821476248748463</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>40148</v>
+      </c>
+      <c r="B37" s="7">
         <v>894068</v>
       </c>
-      <c r="B37">
+      <c r="C37" s="8">
         <v>1115.0999999999999</v>
+      </c>
+      <c r="D37" s="14">
+        <f t="shared" si="0"/>
+        <v>-0.105932</v>
+      </c>
+      <c r="E37" s="15">
+        <f t="shared" si="1"/>
+        <v>-0.22467738346868402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>